<commit_message>
Update File Query and clean code Jpa Repository
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMR004.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="0" windowWidth="22320" windowHeight="13875"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="合計書（職場別）" sheetId="49" r:id="rId1"/>
@@ -169,7 +169,7 @@
     <definedName name="PG単価">[9]明細合計!#REF!</definedName>
     <definedName name="PG田中" localSheetId="0">#REF!</definedName>
     <definedName name="PG田中">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'合計書（職場別）'!$A$1:$J$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'合計書（職場別）'!$A$1:$J$8</definedName>
     <definedName name="PrintDaicho" localSheetId="0">[10]!PrintDaicho</definedName>
     <definedName name="PrintDaicho">[10]!PrintDaicho</definedName>
     <definedName name="QuitDaicho" localSheetId="0">[10]!QuitDaicho</definedName>
@@ -388,51 +388,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>No</t>
-    <phoneticPr fontId="19"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <rPh sb="0" eb="2">
-      <t>メイショウ</t>
-    </rPh>
-    <phoneticPr fontId="19"/>
-  </si>
-  <si>
-    <t>数量</t>
-    <rPh sb="0" eb="2">
-      <t>スウリョウ</t>
-    </rPh>
-    <phoneticPr fontId="19"/>
-  </si>
-  <si>
-    <t>合計</t>
-    <rPh sb="0" eb="2">
-      <t>ゴウケイ</t>
-    </rPh>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>金額</t>
-    <rPh sb="0" eb="2">
-      <t>キンガク</t>
-    </rPh>
-    <phoneticPr fontId="19"/>
-  </si>
-  <si>
-    <t>職場○：</t>
-    <rPh sb="0" eb="2">
-      <t>ショクバ</t>
-    </rPh>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>期間：</t>
-    <phoneticPr fontId="9"/>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -441,7 +397,7 @@
     <numFmt numFmtId="164" formatCode="&quot;¥&quot;#,##0;[Red]&quot;¥&quot;\-#,##0"/>
     <numFmt numFmtId="165" formatCode="\ @"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -581,12 +537,6 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
-    <font>
-      <sz val="6"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -620,7 +570,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -664,15 +614,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="double">
         <color indexed="64"/>
       </top>
@@ -702,19 +643,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="dotted">
         <color indexed="64"/>
@@ -723,17 +651,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -757,58 +674,10 @@
       <left style="dotted">
         <color indexed="64"/>
       </left>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="dotted">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -873,17 +742,6 @@
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -973,7 +831,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1">
       <alignment vertical="center"/>
@@ -984,7 +842,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="18" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -993,83 +851,44 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="16" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="23" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="15" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="9" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="16" fillId="5" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="20" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="13" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="8" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="18" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1077,40 +896,25 @@
     <xf numFmtId="165" fontId="16" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="5" borderId="17" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="5" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="3" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="17" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="19" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="12" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="4" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="4" borderId="4" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
@@ -45207,7 +45011,7 @@
   <sheetPr>
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
   </sheetViews>
@@ -45231,34 +45035,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="A1" s="8"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A2" s="10"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
+      <c r="A2" s="8"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1">
-      <c r="A3" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="48"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
       <c r="D3" s="2"/>
       <c r="F3" s="2"/>
     </row>
@@ -45269,377 +45069,62 @@
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="19.5" customHeight="1" thickBot="1">
-      <c r="D5" s="44" t="s">
-        <v>0</v>
-      </c>
+      <c r="D5" s="26"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="38"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1">
-      <c r="C6" s="17"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="29"/>
       <c r="J6" s="6"/>
     </row>
-    <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="C7" s="17"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="39"/>
+    <row r="7" spans="1:10" ht="15" customHeight="1" thickBot="1">
+      <c r="C7" s="11"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="24"/>
     </row>
-    <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="D8" s="34"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="47"/>
+    <row r="8" spans="1:10" ht="15" customHeight="1" thickTop="1">
+      <c r="D8" s="7"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1">
-      <c r="D9" s="35"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="39"/>
+      <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:10" ht="15" customHeight="1">
-      <c r="D10" s="34"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="47"/>
-    </row>
-    <row r="11" spans="1:10" ht="15" customHeight="1">
-      <c r="D11" s="35"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="39"/>
-    </row>
-    <row r="12" spans="1:10" ht="15" customHeight="1">
-      <c r="D12" s="34"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="47"/>
-    </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1">
-      <c r="D13" s="35"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="39"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1">
-      <c r="D14" s="34"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="47"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="D15" s="35"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="39"/>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1">
-      <c r="D16" s="34"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="47"/>
-    </row>
-    <row r="17" spans="4:14" ht="15" customHeight="1">
-      <c r="D17" s="35"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="39"/>
-    </row>
-    <row r="18" spans="4:14" ht="15" customHeight="1">
-      <c r="D18" s="34"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="47"/>
-    </row>
-    <row r="19" spans="4:14" ht="15" customHeight="1">
-      <c r="D19" s="35"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="39"/>
-    </row>
-    <row r="20" spans="4:14" ht="15" customHeight="1">
-      <c r="D20" s="34"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="47"/>
-    </row>
-    <row r="21" spans="4:14" ht="15" customHeight="1">
-      <c r="D21" s="35"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="39"/>
-    </row>
-    <row r="22" spans="4:14" ht="15" customHeight="1">
-      <c r="D22" s="36"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="4:14" ht="15" customHeight="1">
-      <c r="D23" s="35"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="39"/>
-    </row>
-    <row r="24" spans="4:14" ht="15" customHeight="1">
-      <c r="D24" s="34"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="40"/>
-    </row>
-    <row r="25" spans="4:14" ht="15" customHeight="1">
-      <c r="D25" s="35"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="39"/>
-    </row>
-    <row r="26" spans="4:14" ht="15" customHeight="1">
-      <c r="D26" s="37"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="47"/>
-    </row>
-    <row r="27" spans="4:14" ht="15" customHeight="1">
-      <c r="D27" s="35"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="39"/>
-    </row>
-    <row r="28" spans="4:14" ht="15" customHeight="1">
-      <c r="D28" s="34"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="47"/>
-    </row>
-    <row r="29" spans="4:14" ht="15" customHeight="1">
-      <c r="D29" s="35"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="39"/>
-    </row>
-    <row r="30" spans="4:14" ht="15" customHeight="1">
-      <c r="D30" s="34"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="47"/>
-      <c r="N30" s="7"/>
-    </row>
-    <row r="31" spans="4:14" ht="15" customHeight="1">
-      <c r="D31" s="35"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="39"/>
-    </row>
-    <row r="32" spans="4:14" ht="15" customHeight="1">
-      <c r="D32" s="34"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="41"/>
-    </row>
-    <row r="33" spans="4:9" ht="15" customHeight="1">
-      <c r="D33" s="35"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="39"/>
-    </row>
-    <row r="34" spans="4:9" ht="15" customHeight="1">
-      <c r="D34" s="34"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="47"/>
-    </row>
-    <row r="35" spans="4:9" ht="15" customHeight="1">
-      <c r="D35" s="35"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="39"/>
-    </row>
-    <row r="36" spans="4:9" ht="15" customHeight="1">
-      <c r="D36" s="34"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="28"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="47"/>
-    </row>
-    <row r="37" spans="4:9" ht="15" customHeight="1">
-      <c r="D37" s="35"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="39"/>
-    </row>
-    <row r="38" spans="4:9" ht="15" customHeight="1">
-      <c r="D38" s="34"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="18"/>
-      <c r="I38" s="47"/>
-    </row>
-    <row r="39" spans="4:9" ht="15" customHeight="1">
-      <c r="D39" s="35"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="39"/>
-    </row>
-    <row r="40" spans="4:9" ht="15" customHeight="1">
-      <c r="D40" s="34"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="15"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="47"/>
-    </row>
-    <row r="41" spans="4:9" ht="15" customHeight="1">
-      <c r="D41" s="35"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="39"/>
-    </row>
-    <row r="42" spans="4:9" ht="15" customHeight="1">
-      <c r="D42" s="34"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="15"/>
-      <c r="H42" s="18"/>
-      <c r="I42" s="47"/>
-    </row>
-    <row r="43" spans="4:9" ht="15" customHeight="1">
-      <c r="D43" s="35"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="39"/>
-    </row>
-    <row r="44" spans="4:9" ht="15" customHeight="1">
-      <c r="D44" s="34"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="31"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="18"/>
-      <c r="I44" s="47"/>
-    </row>
-    <row r="45" spans="4:9" ht="15" customHeight="1" thickBot="1">
-      <c r="D45" s="32"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="16"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="42"/>
-    </row>
-    <row r="46" spans="4:9" ht="15" customHeight="1" thickTop="1">
-      <c r="D46" s="9"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G46" s="46"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="23"/>
-    </row>
-    <row r="47" spans="4:9" ht="15" customHeight="1">
-      <c r="F47" s="17"/>
-    </row>
-    <row r="48" spans="4:9" ht="15" customHeight="1"/>
-    <row r="49" ht="15" customHeight="1"/>
-    <row r="50" ht="15" customHeight="1"/>
-    <row r="51" ht="15" customHeight="1"/>
-    <row r="52" ht="15" customHeight="1"/>
-    <row r="53" ht="15" customHeight="1"/>
-    <row r="54" ht="15" customHeight="1"/>
-    <row r="55" ht="15" customHeight="1"/>
-    <row r="56" ht="15" customHeight="1"/>
-    <row r="57" ht="15" customHeight="1"/>
-    <row r="58" ht="15" customHeight="1"/>
-    <row r="59" ht="15" customHeight="1"/>
-    <row r="60" ht="15" customHeight="1"/>
-    <row r="61" ht="15" customHeight="1"/>
-    <row r="62" ht="15" customHeight="1"/>
-    <row r="63" ht="15" customHeight="1"/>
-    <row r="64" ht="15" customHeight="1"/>
-    <row r="65" ht="15" customHeight="1"/>
-    <row r="66" ht="15" customHeight="1"/>
+    <row r="10" spans="1:10" ht="15" customHeight="1"/>
+    <row r="11" spans="1:10" ht="15" customHeight="1"/>
+    <row r="12" spans="1:10" ht="15" customHeight="1"/>
+    <row r="13" spans="1:10" ht="15" customHeight="1"/>
+    <row r="14" spans="1:10" ht="15" customHeight="1"/>
+    <row r="15" spans="1:10" ht="15" customHeight="1"/>
+    <row r="16" spans="1:10" ht="15" customHeight="1"/>
+    <row r="17" ht="15" customHeight="1"/>
+    <row r="18" ht="15" customHeight="1"/>
+    <row r="19" ht="15" customHeight="1"/>
+    <row r="20" ht="15" customHeight="1"/>
+    <row r="21" ht="15" customHeight="1"/>
+    <row r="22" ht="15" customHeight="1"/>
+    <row r="23" ht="15" customHeight="1"/>
+    <row r="24" ht="15" customHeight="1"/>
+    <row r="25" ht="15" customHeight="1"/>
+    <row r="26" ht="15" customHeight="1"/>
+    <row r="27" ht="15" customHeight="1"/>
+    <row r="28" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A3:B3"/>

</xml_diff>